<commit_message>
fix #372 : fixed reading an array from a CSV or Excel file when the columns axis is not explicitly named (via a backslash)
</commit_message>
<xml_diff>
--- a/larray/tests/test.xlsx
+++ b/larray/tests/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12210" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12210" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1d" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="3d" sheetId="3" r:id="rId3"/>
     <sheet name="5d" sheetId="4" r:id="rId4"/>
     <sheet name="missing_values" sheetId="5" r:id="rId5"/>
+    <sheet name="2d_classic" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="9">
   <si>
     <t>time</t>
   </si>
@@ -61,7 +62,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +98,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +456,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,163 +1712,265 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80D36B7-2770-4F08-9EB8-0F661DAA5833}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2007</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3722</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3395</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>338</v>
+      </c>
+      <c r="D3" s="1">
+        <v>316</v>
+      </c>
+      <c r="E3" s="1">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2878</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2791</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2822</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4073</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4161</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4429</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1561</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1463</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3507</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3741</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3366</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2052</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2052</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3785</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3508</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209DDD0A-858D-4DCF-ACE7-9BEBA17CBB59}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
+      <c r="B1">
+        <v>2007</v>
       </c>
       <c r="C1">
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="D1">
-        <v>2010</v>
-      </c>
-      <c r="E1">
         <v>2013</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2">
+        <v>3722</v>
       </c>
       <c r="C2">
-        <v>3722</v>
+        <v>3395</v>
       </c>
       <c r="D2">
-        <v>3395</v>
-      </c>
-      <c r="E2">
         <v>3347</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>338</v>
       </c>
       <c r="C3">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="D3">
-        <v>316</v>
-      </c>
-      <c r="E3">
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2878</v>
       </c>
       <c r="C4">
-        <v>2878</v>
+        <v>2791</v>
       </c>
       <c r="D4">
-        <v>2791</v>
-      </c>
-      <c r="E4">
         <v>2822</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1121</v>
       </c>
       <c r="C5">
+        <v>1037</v>
+      </c>
+      <c r="D5">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>4073</v>
       </c>
-      <c r="D5">
+      <c r="C6">
         <v>4161</v>
       </c>
-      <c r="E5">
+      <c r="D6">
         <v>4429</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>1561</v>
-      </c>
-      <c r="D6">
-        <v>1463</v>
-      </c>
-      <c r="E6">
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>3507</v>
-      </c>
-      <c r="D7">
-        <v>3741</v>
-      </c>
-      <c r="E7">
-        <v>3366</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>2052</v>
-      </c>
-      <c r="D8">
-        <v>2052</v>
-      </c>
-      <c r="E8">
-        <v>2118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>3785</v>
-      </c>
-      <c r="D9">
-        <v>3508</v>
-      </c>
-      <c r="E9">
-        <v>3172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix #393 : allowed to use arguments fill_value, sort_columns and sort_rows from read_excel in case engine=xlwings
</commit_message>
<xml_diff>
--- a/larray/tests/test.xlsx
+++ b/larray/tests/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12210" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1d" sheetId="1" r:id="rId1"/>
     <sheet name="2d" sheetId="2" r:id="rId2"/>
     <sheet name="3d" sheetId="3" r:id="rId3"/>
     <sheet name="5d" sheetId="4" r:id="rId4"/>
+    <sheet name="missing_values" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="9">
   <si>
     <t>time</t>
   </si>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,7 +405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -442,10 +443,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -539,10 +542,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -739,10 +744,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1692,4 +1697,172 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80D36B7-2770-4F08-9EB8-0F661DAA5833}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1">
+        <v>2007</v>
+      </c>
+      <c r="D1">
+        <v>2010</v>
+      </c>
+      <c r="E1">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>3722</v>
+      </c>
+      <c r="D2">
+        <v>3395</v>
+      </c>
+      <c r="E2">
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>338</v>
+      </c>
+      <c r="D3">
+        <v>316</v>
+      </c>
+      <c r="E3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2878</v>
+      </c>
+      <c r="D4">
+        <v>2791</v>
+      </c>
+      <c r="E4">
+        <v>2822</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4073</v>
+      </c>
+      <c r="D5">
+        <v>4161</v>
+      </c>
+      <c r="E5">
+        <v>4429</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1561</v>
+      </c>
+      <c r="D6">
+        <v>1463</v>
+      </c>
+      <c r="E6">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>3507</v>
+      </c>
+      <c r="D7">
+        <v>3741</v>
+      </c>
+      <c r="E7">
+        <v>3366</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>2052</v>
+      </c>
+      <c r="D8">
+        <v>2052</v>
+      </c>
+      <c r="E8">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>3785</v>
+      </c>
+      <c r="D9">
+        <v>3508</v>
+      </c>
+      <c r="E9">
+        <v>3172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix #393 : support arguments fill_value, sort_columns and sort_rows in read_excel with xlwings (#435)
fix #393 : allowed to use arguments fill_value, sort_columns and sort_rows from read_excel in case engine=xlwings
</commit_message>
<xml_diff>
--- a/larray/tests/test.xlsx
+++ b/larray/tests/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12210" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1d" sheetId="1" r:id="rId1"/>
     <sheet name="2d" sheetId="2" r:id="rId2"/>
     <sheet name="3d" sheetId="3" r:id="rId3"/>
     <sheet name="5d" sheetId="4" r:id="rId4"/>
+    <sheet name="missing_values" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="9">
   <si>
     <t>time</t>
   </si>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,7 +405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -442,10 +443,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -539,10 +542,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -739,10 +744,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1692,4 +1697,172 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80D36B7-2770-4F08-9EB8-0F661DAA5833}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1">
+        <v>2007</v>
+      </c>
+      <c r="D1">
+        <v>2010</v>
+      </c>
+      <c r="E1">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>3722</v>
+      </c>
+      <c r="D2">
+        <v>3395</v>
+      </c>
+      <c r="E2">
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>338</v>
+      </c>
+      <c r="D3">
+        <v>316</v>
+      </c>
+      <c r="E3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2878</v>
+      </c>
+      <c r="D4">
+        <v>2791</v>
+      </c>
+      <c r="E4">
+        <v>2822</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4073</v>
+      </c>
+      <c r="D5">
+        <v>4161</v>
+      </c>
+      <c r="E5">
+        <v>4429</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1561</v>
+      </c>
+      <c r="D6">
+        <v>1463</v>
+      </c>
+      <c r="E6">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>3507</v>
+      </c>
+      <c r="D7">
+        <v>3741</v>
+      </c>
+      <c r="E7">
+        <v>3366</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>2052</v>
+      </c>
+      <c r="D8">
+        <v>2052</v>
+      </c>
+      <c r="E8">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>3785</v>
+      </c>
+      <c r="D9">
+        <v>3508</v>
+      </c>
+      <c r="E9">
+        <v>3172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>